<commit_message>
Completed baseline model and MLP model tests
</commit_message>
<xml_diff>
--- a/src/models/baseline_lr_model_results.xlsx
+++ b/src/models/baseline_lr_model_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCL_CS\Y3\COMP0029 Individual Project\Individual Project (90%)\UCL-FYP\src\baseline_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCL_CS\Y3\COMP0029 Individual Project\Individual Project (90%)\UCL-FYP\src\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FCB3B4-6586-4C95-B164-1B6AFB1535F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9DF908-F050-410D-BB6D-7C4C2346C7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18930" yWindow="3420" windowWidth="14295" windowHeight="10875" xr2:uid="{449CD272-F864-49D6-AEEE-8295C86900CF}"/>
+    <workbookView xWindow="-25395" yWindow="1995" windowWidth="14295" windowHeight="10875" xr2:uid="{449CD272-F864-49D6-AEEE-8295C86900CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,13 +579,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="4">
-        <v>72.5</v>
+        <v>80</v>
       </c>
       <c r="E7" s="4">
-        <v>92.5</v>
+        <v>80</v>
       </c>
       <c r="F7" s="4">
-        <v>92.5</v>
+        <v>80</v>
       </c>
       <c r="G7" s="4">
         <v>75</v>
@@ -594,16 +594,16 @@
         <v>67.5</v>
       </c>
       <c r="I7" s="4">
-        <v>82.5</v>
+        <v>77.5</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="4">
-        <v>95</v>
+        <v>87.5</v>
       </c>
       <c r="L7" s="4">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">

</xml_diff>